<commit_message>
added rank movement feature, changed directory structure and various script enhancements
</commit_message>
<xml_diff>
--- a/final/leaderboard.xlsx
+++ b/final/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meInspiron\Desktop\ipl_polls\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DC7739-009E-4461-A85F-219569AD09B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69FFF04-132A-4CC5-9361-36850B784984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{33315BC7-FE13-4B47-AD11-5FFBB64D564A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="245">
   <si>
     <t>Username</t>
   </si>
@@ -1439,6 +1439,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1514,60 +1554,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1575,35 +1566,44 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1611,16 +1611,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1691,6 +1681,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2049,575 +2049,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2955,7 +2386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA97E823-CE46-454B-9E87-F5C2FCA41BF0}">
   <dimension ref="B1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -2970,61 +2401,61 @@
   <sheetData>
     <row r="1" spans="2:10" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:10" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="81" t="s">
+      <c r="D2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="38" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="63" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="36">
         <v>5</v>
       </c>
-      <c r="G3" s="76">
+      <c r="G3" s="36">
         <v>7</v>
       </c>
-      <c r="H3" s="76">
+      <c r="H3" s="36">
         <v>10</v>
       </c>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76">
+      <c r="I3" s="36"/>
+      <c r="J3" s="36">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="51" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="22" t="s">
         <v>75</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -3045,9 +2476,9 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="51" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="22" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -3068,9 +2499,9 @@
       </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="51" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="22" t="s">
         <v>105</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -3091,9 +2522,9 @@
       </c>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="51" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="22" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -3114,9 +2545,9 @@
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="51" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="22" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -3137,9 +2568,9 @@
       </c>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="51" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="22" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -3160,9 +2591,9 @@
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="51" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="22" t="s">
         <v>99</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -3183,9 +2614,9 @@
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="51" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="22" t="s">
         <v>122</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -3206,9 +2637,9 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="51" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -3229,9 +2660,9 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="51" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="22" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="11"/>
@@ -3250,9 +2681,9 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="51" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="22" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -3273,9 +2704,9 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="51" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="22" t="s">
         <v>69</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -3296,9 +2727,9 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="51" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="22" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -3319,9 +2750,9 @@
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="51" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="22" t="s">
         <v>65</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -3342,9 +2773,9 @@
       </c>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="51" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -3365,9 +2796,9 @@
       </c>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="51" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="22" t="s">
         <v>97</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -3388,9 +2819,9 @@
       </c>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="51" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="22" t="s">
         <v>117</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -3411,9 +2842,9 @@
       </c>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="51" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="22" t="s">
         <v>124</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -3434,9 +2865,9 @@
       </c>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="51" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="22" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -3457,9 +2888,9 @@
       </c>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="51" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="22" t="s">
         <v>80</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -3480,9 +2911,9 @@
       </c>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="51" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="22" t="s">
         <v>95</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -3503,9 +2934,9 @@
       </c>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="51" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="22" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -3526,9 +2957,9 @@
       </c>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="51" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="22" t="s">
         <v>93</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -3549,9 +2980,9 @@
       </c>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="51" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="22" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -3572,9 +3003,9 @@
       </c>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="51" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -3595,9 +3026,9 @@
       </c>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="51" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="22" t="s">
         <v>71</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -3618,9 +3049,9 @@
       </c>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="51" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -3641,9 +3072,9 @@
       </c>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="51" t="s">
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="22" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -3664,9 +3095,9 @@
       </c>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="51" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -3687,9 +3118,9 @@
       </c>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="51" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="22" t="s">
         <v>113</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -3710,9 +3141,9 @@
       </c>
     </row>
     <row r="34" spans="2:10">
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="51" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="22" t="s">
         <v>182</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -3733,9 +3164,9 @@
       </c>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="51" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="22" t="s">
         <v>164</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -3756,9 +3187,9 @@
       </c>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="51" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="22" t="s">
         <v>210</v>
       </c>
       <c r="E36" s="11" t="s">
@@ -3779,9 +3210,9 @@
       </c>
     </row>
     <row r="37" spans="2:10">
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="51" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E37" s="11" t="s">
@@ -3802,9 +3233,9 @@
       </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="51" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="22" t="s">
         <v>89</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -3825,9 +3256,9 @@
       </c>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="51" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="22" t="s">
         <v>78</v>
       </c>
       <c r="E39" s="11" t="s">
@@ -3848,9 +3279,9 @@
       </c>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="51" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="22" t="s">
         <v>42</v>
       </c>
       <c r="E40" s="11"/>
@@ -3869,9 +3300,9 @@
       </c>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="51" t="s">
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="22" t="s">
         <v>154</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -3892,9 +3323,9 @@
       </c>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="51" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="22" t="s">
         <v>111</v>
       </c>
       <c r="E42" s="11" t="s">
@@ -3915,9 +3346,9 @@
       </c>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="51" t="s">
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="22" t="s">
         <v>83</v>
       </c>
       <c r="E43" s="11" t="s">
@@ -3938,9 +3369,9 @@
       </c>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="59"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="51" t="s">
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="22" t="s">
         <v>156</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -3961,9 +3392,9 @@
       </c>
     </row>
     <row r="45" spans="2:10">
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="51" t="s">
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="22" t="s">
         <v>53</v>
       </c>
       <c r="E45" s="11"/>
@@ -3982,9 +3413,9 @@
       </c>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="51" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="22" t="s">
         <v>166</v>
       </c>
       <c r="E46" s="11" t="s">
@@ -4005,9 +3436,9 @@
       </c>
     </row>
     <row r="47" spans="2:10">
-      <c r="B47" s="59"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="51" t="s">
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="22" t="s">
         <v>130</v>
       </c>
       <c r="E47" s="11" t="s">
@@ -4028,9 +3459,9 @@
       </c>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="59"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="51" t="s">
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="22" t="s">
         <v>85</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -4051,9 +3482,9 @@
       </c>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="51" t="s">
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="22" t="s">
         <v>180</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -4074,9 +3505,9 @@
       </c>
     </row>
     <row r="50" spans="2:10">
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="51" t="s">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="22" t="s">
         <v>212</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -4097,9 +3528,9 @@
       </c>
     </row>
     <row r="51" spans="2:10">
-      <c r="B51" s="59"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="51" t="s">
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="22" t="s">
         <v>214</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -4120,9 +3551,9 @@
       </c>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="59"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="51" t="s">
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="22" t="s">
         <v>216</v>
       </c>
       <c r="E52" s="11"/>
@@ -4141,9 +3572,9 @@
       </c>
     </row>
     <row r="53" spans="2:10">
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="51" t="s">
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="22" t="s">
         <v>217</v>
       </c>
       <c r="E53" s="11" t="s">
@@ -4164,9 +3595,9 @@
       </c>
     </row>
     <row r="54" spans="2:10">
-      <c r="B54" s="59"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="51" t="s">
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="22" t="s">
         <v>120</v>
       </c>
       <c r="E54" s="11" t="s">
@@ -4187,9 +3618,9 @@
       </c>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="59"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="51" t="s">
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="22" t="s">
         <v>24</v>
       </c>
       <c r="E55" s="11" t="s">
@@ -4210,9 +3641,9 @@
       </c>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="59"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="51" t="s">
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E56" s="11" t="s">
@@ -4233,9 +3664,9 @@
       </c>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="59"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="51" t="s">
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="22" t="s">
         <v>40</v>
       </c>
       <c r="E57" s="11" t="s">
@@ -4256,9 +3687,9 @@
       </c>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="51" t="s">
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="22" t="s">
         <v>47</v>
       </c>
       <c r="E58" s="11" t="s">
@@ -4279,9 +3710,9 @@
       </c>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="51" t="s">
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="22" t="s">
         <v>51</v>
       </c>
       <c r="E59" s="11" t="s">
@@ -4302,9 +3733,9 @@
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="51" t="s">
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E60" s="11" t="s">
@@ -4325,9 +3756,9 @@
       </c>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" s="59"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="51" t="s">
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="22" t="s">
         <v>103</v>
       </c>
       <c r="E61" s="11" t="s">
@@ -4348,9 +3779,9 @@
       </c>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="59"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="51" t="s">
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="22" t="s">
         <v>158</v>
       </c>
       <c r="E62" s="11" t="s">
@@ -4371,9 +3802,9 @@
       </c>
     </row>
     <row r="63" spans="2:10">
-      <c r="B63" s="59"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="51" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="22" t="s">
         <v>160</v>
       </c>
       <c r="E63" s="11" t="s">
@@ -4394,9 +3825,9 @@
       </c>
     </row>
     <row r="64" spans="2:10">
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="51" t="s">
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="22" t="s">
         <v>162</v>
       </c>
       <c r="E64" s="11" t="s">
@@ -4417,9 +3848,9 @@
       </c>
     </row>
     <row r="65" spans="2:10">
-      <c r="B65" s="59"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="51" t="s">
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="22" t="s">
         <v>168</v>
       </c>
       <c r="E65" s="11" t="s">
@@ -4440,9 +3871,9 @@
       </c>
     </row>
     <row r="66" spans="2:10">
-      <c r="B66" s="59"/>
-      <c r="C66" s="59"/>
-      <c r="D66" s="51" t="s">
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="22" t="s">
         <v>176</v>
       </c>
       <c r="E66" s="11" t="s">
@@ -4463,9 +3894,9 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="B67" s="59"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="51" t="s">
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="22" t="s">
         <v>132</v>
       </c>
       <c r="E67" s="11" t="s">
@@ -4486,9 +3917,9 @@
       </c>
     </row>
     <row r="68" spans="2:10">
-      <c r="B68" s="59"/>
-      <c r="C68" s="59"/>
-      <c r="D68" s="51" t="s">
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E68" s="11" t="s">
@@ -4509,9 +3940,9 @@
       </c>
     </row>
     <row r="69" spans="2:10">
-      <c r="B69" s="59"/>
-      <c r="C69" s="59"/>
-      <c r="D69" s="51" t="s">
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="22" t="s">
         <v>22</v>
       </c>
       <c r="E69" s="11" t="s">
@@ -4532,9 +3963,9 @@
       </c>
     </row>
     <row r="70" spans="2:10">
-      <c r="B70" s="59"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="51" t="s">
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="22" t="s">
         <v>35</v>
       </c>
       <c r="E70" s="11" t="s">
@@ -4555,9 +3986,9 @@
       </c>
     </row>
     <row r="71" spans="2:10">
-      <c r="B71" s="59"/>
-      <c r="C71" s="59"/>
-      <c r="D71" s="51" t="s">
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E71" s="11" t="s">
@@ -4578,9 +4009,9 @@
       </c>
     </row>
     <row r="72" spans="2:10">
-      <c r="B72" s="59"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="51" t="s">
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="22" t="s">
         <v>62</v>
       </c>
       <c r="E72" s="11" t="s">
@@ -4601,9 +4032,9 @@
       </c>
     </row>
     <row r="73" spans="2:10">
-      <c r="B73" s="59"/>
-      <c r="C73" s="59"/>
-      <c r="D73" s="51" t="s">
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="22" t="s">
         <v>109</v>
       </c>
       <c r="E73" s="11" t="s">
@@ -4624,9 +4055,9 @@
       </c>
     </row>
     <row r="74" spans="2:10">
-      <c r="B74" s="59"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="51" t="s">
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="22" t="s">
         <v>118</v>
       </c>
       <c r="E74" s="11" t="s">
@@ -4647,9 +4078,9 @@
       </c>
     </row>
     <row r="75" spans="2:10">
-      <c r="B75" s="59"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="51" t="s">
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="22" t="s">
         <v>115</v>
       </c>
       <c r="E75" s="11" t="s">
@@ -4670,9 +4101,9 @@
       </c>
     </row>
     <row r="76" spans="2:10">
-      <c r="B76" s="59"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="51" t="s">
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="22" t="s">
         <v>170</v>
       </c>
       <c r="E76" s="11" t="s">
@@ -4693,9 +4124,9 @@
       </c>
     </row>
     <row r="77" spans="2:10">
-      <c r="B77" s="59"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="51" t="s">
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="22" t="s">
         <v>172</v>
       </c>
       <c r="E77" s="11" t="s">
@@ -4716,9 +4147,9 @@
       </c>
     </row>
     <row r="78" spans="2:10">
-      <c r="B78" s="59"/>
-      <c r="C78" s="59"/>
-      <c r="D78" s="51" t="s">
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="22" t="s">
         <v>174</v>
       </c>
       <c r="E78" s="11" t="s">
@@ -4739,9 +4170,9 @@
       </c>
     </row>
     <row r="79" spans="2:10">
-      <c r="B79" s="59"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="51" t="s">
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="22" t="s">
         <v>178</v>
       </c>
       <c r="E79" s="11" t="s">
@@ -4762,9 +4193,9 @@
       </c>
     </row>
     <row r="80" spans="2:10">
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="51" t="s">
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="22" t="s">
         <v>184</v>
       </c>
       <c r="E80" s="11" t="s">
@@ -4785,9 +4216,9 @@
       </c>
     </row>
     <row r="81" spans="2:10">
-      <c r="B81" s="59"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="51" t="s">
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="22" t="s">
         <v>219</v>
       </c>
       <c r="E81" s="11" t="s">
@@ -4808,9 +4239,9 @@
       </c>
     </row>
     <row r="82" spans="2:10" ht="15" thickBot="1">
-      <c r="B82" s="60"/>
-      <c r="C82" s="60"/>
-      <c r="D82" s="52" t="s">
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="23" t="s">
         <v>221</v>
       </c>
       <c r="E82" s="12" t="s">
@@ -4831,7 +4262,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:J100">
+  <conditionalFormatting sqref="B3:J150">
     <cfRule type="expression" dxfId="45" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -4873,121 +4304,121 @@
   <sheetData>
     <row r="1" spans="2:18" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="40"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="2:18" ht="15">
-      <c r="B3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="36" t="s">
+      <c r="O3" s="45"/>
+      <c r="P3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="42" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15">
-      <c r="B4" s="31"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="47"/>
+      <c r="F4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="47"/>
+      <c r="J4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="36"/>
-      <c r="R4" s="23"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="56"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B5" s="32"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="52"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="49"/>
+      <c r="F5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="28" t="s">
+      <c r="I5" s="49"/>
+      <c r="J5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="49"/>
+      <c r="L5" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="28" t="s">
+      <c r="M5" s="49"/>
+      <c r="N5" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="37"/>
-      <c r="R5" s="23"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="57"/>
+      <c r="R5" s="43"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
@@ -8060,149 +7491,149 @@
   <sheetData>
     <row r="1" spans="2:22" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="61" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="43"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="63"/>
     </row>
     <row r="3" spans="2:22" ht="15" customHeight="1">
-      <c r="B3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="24" t="s">
+      <c r="O3" s="45"/>
+      <c r="P3" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="45"/>
+      <c r="R3" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="44" t="s">
+      <c r="S3" s="45"/>
+      <c r="T3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="42" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15">
-      <c r="B4" s="31"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="47"/>
+      <c r="F4" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="47"/>
+      <c r="J4" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="26" t="s">
+      <c r="O4" s="47"/>
+      <c r="P4" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="26" t="s">
+      <c r="Q4" s="47"/>
+      <c r="R4" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="45"/>
-      <c r="V4" s="23"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="65"/>
+      <c r="V4" s="43"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B5" s="32"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="52"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="49"/>
+      <c r="F5" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="28" t="s">
+      <c r="I5" s="49"/>
+      <c r="J5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="49"/>
+      <c r="L5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="28" t="s">
+      <c r="M5" s="49"/>
+      <c r="N5" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="28" t="s">
+      <c r="O5" s="49"/>
+      <c r="P5" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="28" t="s">
+      <c r="Q5" s="49"/>
+      <c r="R5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="46"/>
-      <c r="V5" s="23"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="66"/>
+      <c r="V5" s="43"/>
     </row>
     <row r="6" spans="2:22">
       <c r="B6" s="14" t="s">
@@ -11669,177 +11100,177 @@
   <sheetData>
     <row r="1" spans="2:26" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="61" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="43"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:26" ht="15" customHeight="1">
-      <c r="B3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="24" t="s">
+      <c r="O3" s="45"/>
+      <c r="P3" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="45"/>
+      <c r="R3" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24" t="s">
+      <c r="S3" s="45"/>
+      <c r="T3" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="24" t="s">
+      <c r="U3" s="45"/>
+      <c r="V3" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="W3" s="25"/>
-      <c r="X3" s="44" t="s">
+      <c r="W3" s="45"/>
+      <c r="X3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="22" t="s">
+      <c r="Z3" s="42" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="15">
-      <c r="B4" s="31"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="47"/>
+      <c r="F4" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="47"/>
+      <c r="J4" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="26" t="s">
+      <c r="O4" s="47"/>
+      <c r="P4" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="26" t="s">
+      <c r="Q4" s="47"/>
+      <c r="R4" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="26" t="s">
+      <c r="S4" s="47"/>
+      <c r="T4" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="26" t="s">
+      <c r="U4" s="47"/>
+      <c r="V4" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="27"/>
-      <c r="X4" s="45"/>
-      <c r="Z4" s="23"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="65"/>
+      <c r="Z4" s="43"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B5" s="32"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="28" t="s">
+      <c r="B5" s="52"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="49"/>
+      <c r="F5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="28" t="s">
+      <c r="I5" s="49"/>
+      <c r="J5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="49"/>
+      <c r="L5" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="28" t="s">
+      <c r="M5" s="49"/>
+      <c r="N5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="28" t="s">
+      <c r="O5" s="49"/>
+      <c r="P5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="28" t="s">
+      <c r="Q5" s="49"/>
+      <c r="R5" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="29"/>
-      <c r="T5" s="28" t="s">
+      <c r="S5" s="49"/>
+      <c r="T5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="U5" s="29"/>
-      <c r="V5" s="28" t="s">
+      <c r="U5" s="49"/>
+      <c r="V5" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="W5" s="29"/>
-      <c r="X5" s="46"/>
-      <c r="Z5" s="23"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="66"/>
+      <c r="Z5" s="43"/>
     </row>
     <row r="6" spans="2:26">
       <c r="B6" s="14" t="s">
@@ -15672,6 +15103,12 @@
     <filterColumn colId="20" showButton="0"/>
   </autoFilter>
   <mergeCells count="35">
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="T5:U5"/>
     <mergeCell ref="B2:X2"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
@@ -15685,9 +15122,9 @@
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
     <mergeCell ref="Z3:Z5"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -15701,12 +15138,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C194 X6:X194">
     <cfRule type="expression" dxfId="24" priority="46">
@@ -15783,7 +15214,7 @@
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="V5" sqref="V5:W5"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15815,191 +15246,195 @@
   <sheetData>
     <row r="1" spans="2:26" ht="5.25" customHeight="1"/>
     <row r="2" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="48"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="75"/>
     </row>
     <row r="3" spans="2:26" ht="15" customHeight="1">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="79" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="76" t="s">
         <v>243</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="24" t="s">
+      <c r="D3" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="45"/>
+      <c r="J3" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24" t="s">
+      <c r="K3" s="45"/>
+      <c r="L3" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="M3" s="45"/>
+      <c r="N3" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="24" t="s">
+      <c r="O3" s="45"/>
+      <c r="P3" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="45"/>
+      <c r="R3" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24" t="s">
+      <c r="S3" s="45"/>
+      <c r="T3" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="24" t="s">
+      <c r="U3" s="45"/>
+      <c r="V3" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="W3" s="25"/>
-      <c r="X3" s="69" t="s">
+      <c r="W3" s="45"/>
+      <c r="X3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="22" t="s">
+      <c r="Z3" s="42" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="15">
-      <c r="B4" s="54"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="26" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="47"/>
+      <c r="J4" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="47"/>
+      <c r="N4" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="26" t="s">
+      <c r="O4" s="47"/>
+      <c r="P4" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="26" t="s">
+      <c r="Q4" s="47"/>
+      <c r="R4" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="26" t="s">
+      <c r="S4" s="47"/>
+      <c r="T4" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="26" t="s">
+      <c r="U4" s="47"/>
+      <c r="V4" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="W4" s="27"/>
-      <c r="X4" s="45"/>
-      <c r="Z4" s="23"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="65"/>
+      <c r="Z4" s="43"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="75"/>
-      <c r="T5" s="74"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="46"/>
-      <c r="Z5" s="23"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="73"/>
+      <c r="H5" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" s="73"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="72"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="73"/>
+      <c r="X5" s="66"/>
+      <c r="Z5" s="43"/>
     </row>
     <row r="6" spans="2:26">
-      <c r="B6" s="61"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="68"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="35"/>
       <c r="Z6" s="20">
         <f t="shared" ref="Z6:Z56" si="0">COUNTIF(F6:U6,"---")</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:26">
-      <c r="B7" s="55"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="11"/>
       <c r="F7" s="8"/>
       <c r="G7" s="3"/>
@@ -16026,9 +15461,9 @@
       </c>
     </row>
     <row r="8" spans="2:26">
-      <c r="B8" s="55"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="51"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="11"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -16055,9 +15490,9 @@
       </c>
     </row>
     <row r="9" spans="2:26">
-      <c r="B9" s="55"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="51"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="11"/>
       <c r="F9" s="8"/>
       <c r="G9" s="3"/>
@@ -16084,9 +15519,9 @@
       </c>
     </row>
     <row r="10" spans="2:26">
-      <c r="B10" s="55"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="51"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
       <c r="G10" s="3"/>
@@ -16113,9 +15548,9 @@
       </c>
     </row>
     <row r="11" spans="2:26">
-      <c r="B11" s="55"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="51"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="11"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
@@ -16142,9 +15577,9 @@
       </c>
     </row>
     <row r="12" spans="2:26">
-      <c r="B12" s="55"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="51"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="11"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
@@ -16171,9 +15606,9 @@
       </c>
     </row>
     <row r="13" spans="2:26">
-      <c r="B13" s="55"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="51"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="11"/>
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
@@ -16200,9 +15635,9 @@
       </c>
     </row>
     <row r="14" spans="2:26">
-      <c r="B14" s="55"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="51"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="11"/>
       <c r="F14" s="8"/>
       <c r="G14" s="3"/>
@@ -16229,9 +15664,9 @@
       </c>
     </row>
     <row r="15" spans="2:26">
-      <c r="B15" s="55"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="11"/>
       <c r="F15" s="8"/>
       <c r="G15" s="3"/>
@@ -16258,9 +15693,9 @@
       </c>
     </row>
     <row r="16" spans="2:26">
-      <c r="B16" s="55"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="11"/>
       <c r="F16" s="8"/>
       <c r="G16" s="3"/>
@@ -16287,9 +15722,9 @@
       </c>
     </row>
     <row r="17" spans="2:26">
-      <c r="B17" s="55"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="11"/>
       <c r="F17" s="8"/>
       <c r="G17" s="3"/>
@@ -16316,9 +15751,9 @@
       </c>
     </row>
     <row r="18" spans="2:26">
-      <c r="B18" s="55"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="51"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="11"/>
       <c r="F18" s="8"/>
       <c r="G18" s="3"/>
@@ -16345,9 +15780,9 @@
       </c>
     </row>
     <row r="19" spans="2:26">
-      <c r="B19" s="55"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="51"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="11"/>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
@@ -16374,9 +15809,9 @@
       </c>
     </row>
     <row r="20" spans="2:26">
-      <c r="B20" s="55"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="51"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="11"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
@@ -16403,9 +15838,9 @@
       </c>
     </row>
     <row r="21" spans="2:26">
-      <c r="B21" s="55"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="11"/>
       <c r="F21" s="8"/>
       <c r="G21" s="3"/>
@@ -16432,9 +15867,9 @@
       </c>
     </row>
     <row r="22" spans="2:26">
-      <c r="B22" s="55"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="11"/>
       <c r="F22" s="8"/>
       <c r="G22" s="3"/>
@@ -16461,9 +15896,9 @@
       </c>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="55"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="11"/>
       <c r="F23" s="8"/>
       <c r="G23" s="3"/>
@@ -16490,9 +15925,9 @@
       </c>
     </row>
     <row r="24" spans="2:26">
-      <c r="B24" s="55"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="51"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="11"/>
       <c r="F24" s="8"/>
       <c r="G24" s="3"/>
@@ -16519,9 +15954,9 @@
       </c>
     </row>
     <row r="25" spans="2:26">
-      <c r="B25" s="55"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="11"/>
       <c r="F25" s="8"/>
       <c r="G25" s="3"/>
@@ -16548,9 +15983,9 @@
       </c>
     </row>
     <row r="26" spans="2:26">
-      <c r="B26" s="55"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="51"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="11"/>
       <c r="F26" s="8"/>
       <c r="G26" s="3"/>
@@ -16577,9 +16012,9 @@
       </c>
     </row>
     <row r="27" spans="2:26">
-      <c r="B27" s="55"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="51"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="11"/>
       <c r="F27" s="8"/>
       <c r="G27" s="3"/>
@@ -16606,9 +16041,9 @@
       </c>
     </row>
     <row r="28" spans="2:26">
-      <c r="B28" s="55"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="51"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="11"/>
       <c r="F28" s="8"/>
       <c r="G28" s="3"/>
@@ -16635,9 +16070,9 @@
       </c>
     </row>
     <row r="29" spans="2:26">
-      <c r="B29" s="55"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="51"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="11"/>
       <c r="F29" s="8"/>
       <c r="G29" s="3"/>
@@ -16664,9 +16099,9 @@
       </c>
     </row>
     <row r="30" spans="2:26">
-      <c r="B30" s="55"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="51"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="11"/>
       <c r="F30" s="2"/>
       <c r="G30" s="3"/>
@@ -16693,9 +16128,9 @@
       </c>
     </row>
     <row r="31" spans="2:26">
-      <c r="B31" s="55"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="51"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="11"/>
       <c r="F31" s="2"/>
       <c r="G31" s="3"/>
@@ -16722,9 +16157,9 @@
       </c>
     </row>
     <row r="32" spans="2:26">
-      <c r="B32" s="55"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="51"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="11"/>
       <c r="F32" s="2"/>
       <c r="G32" s="3"/>
@@ -16751,9 +16186,9 @@
       </c>
     </row>
     <row r="33" spans="2:26">
-      <c r="B33" s="55"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="51"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
       <c r="G33" s="3"/>
@@ -16780,9 +16215,9 @@
       </c>
     </row>
     <row r="34" spans="2:26">
-      <c r="B34" s="55"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="11"/>
       <c r="F34" s="8"/>
       <c r="G34" s="3"/>
@@ -16809,9 +16244,9 @@
       </c>
     </row>
     <row r="35" spans="2:26">
-      <c r="B35" s="55"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="51"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="11"/>
       <c r="F35" s="8"/>
       <c r="G35" s="3"/>
@@ -16838,9 +16273,9 @@
       </c>
     </row>
     <row r="36" spans="2:26">
-      <c r="B36" s="55"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="51"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="11"/>
       <c r="F36" s="8"/>
       <c r="G36" s="3"/>
@@ -16867,9 +16302,9 @@
       </c>
     </row>
     <row r="37" spans="2:26">
-      <c r="B37" s="55"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="51"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="11"/>
       <c r="F37" s="8"/>
       <c r="G37" s="3"/>
@@ -16896,9 +16331,9 @@
       </c>
     </row>
     <row r="38" spans="2:26">
-      <c r="B38" s="55"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="51"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="11"/>
       <c r="F38" s="8"/>
       <c r="G38" s="3"/>
@@ -16925,9 +16360,9 @@
       </c>
     </row>
     <row r="39" spans="2:26">
-      <c r="B39" s="55"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="51"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="11"/>
       <c r="F39" s="8"/>
       <c r="G39" s="3"/>
@@ -16954,9 +16389,9 @@
       </c>
     </row>
     <row r="40" spans="2:26">
-      <c r="B40" s="55"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="51"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="11"/>
       <c r="F40" s="8"/>
       <c r="G40" s="3"/>
@@ -16983,9 +16418,9 @@
       </c>
     </row>
     <row r="41" spans="2:26">
-      <c r="B41" s="55"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="51"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="22"/>
       <c r="E41" s="11"/>
       <c r="F41" s="8"/>
       <c r="G41" s="3"/>
@@ -17012,9 +16447,9 @@
       </c>
     </row>
     <row r="42" spans="2:26">
-      <c r="B42" s="55"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="51"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="11"/>
       <c r="F42" s="8"/>
       <c r="G42" s="3"/>
@@ -17041,9 +16476,9 @@
       </c>
     </row>
     <row r="43" spans="2:26">
-      <c r="B43" s="55"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="51"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="11"/>
       <c r="F43" s="8"/>
       <c r="G43" s="3"/>
@@ -17070,9 +16505,9 @@
       </c>
     </row>
     <row r="44" spans="2:26">
-      <c r="B44" s="55"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="51"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="11"/>
       <c r="F44" s="8"/>
       <c r="G44" s="3"/>
@@ -17099,9 +16534,9 @@
       </c>
     </row>
     <row r="45" spans="2:26">
-      <c r="B45" s="55"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="51"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="11"/>
       <c r="F45" s="8"/>
       <c r="G45" s="3"/>
@@ -17128,9 +16563,9 @@
       </c>
     </row>
     <row r="46" spans="2:26">
-      <c r="B46" s="55"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="51"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="22"/>
       <c r="E46" s="11"/>
       <c r="F46" s="8"/>
       <c r="G46" s="3"/>
@@ -17157,9 +16592,9 @@
       </c>
     </row>
     <row r="47" spans="2:26">
-      <c r="B47" s="55"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="51"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="11"/>
       <c r="F47" s="8"/>
       <c r="G47" s="3"/>
@@ -17186,9 +16621,9 @@
       </c>
     </row>
     <row r="48" spans="2:26">
-      <c r="B48" s="55"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="51"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="11"/>
       <c r="F48" s="8"/>
       <c r="G48" s="3"/>
@@ -17215,9 +16650,9 @@
       </c>
     </row>
     <row r="49" spans="2:26">
-      <c r="B49" s="55"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="51"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="11"/>
       <c r="F49" s="8"/>
       <c r="G49" s="3"/>
@@ -17244,9 +16679,9 @@
       </c>
     </row>
     <row r="50" spans="2:26">
-      <c r="B50" s="55"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="51"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="11"/>
       <c r="F50" s="8"/>
       <c r="G50" s="3"/>
@@ -17273,9 +16708,9 @@
       </c>
     </row>
     <row r="51" spans="2:26">
-      <c r="B51" s="55"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="51"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="11"/>
       <c r="F51" s="8"/>
       <c r="G51" s="3"/>
@@ -17302,9 +16737,9 @@
       </c>
     </row>
     <row r="52" spans="2:26">
-      <c r="B52" s="55"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="51"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="11"/>
       <c r="F52" s="8"/>
       <c r="G52" s="3"/>
@@ -17331,9 +16766,9 @@
       </c>
     </row>
     <row r="53" spans="2:26">
-      <c r="B53" s="55"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="51"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="22"/>
       <c r="E53" s="11"/>
       <c r="F53" s="8"/>
       <c r="G53" s="3"/>
@@ -17360,9 +16795,9 @@
       </c>
     </row>
     <row r="54" spans="2:26">
-      <c r="B54" s="55"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="51"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="22"/>
       <c r="E54" s="11"/>
       <c r="F54" s="8"/>
       <c r="G54" s="3"/>
@@ -17389,9 +16824,9 @@
       </c>
     </row>
     <row r="55" spans="2:26">
-      <c r="B55" s="55"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="51"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="22"/>
       <c r="E55" s="11"/>
       <c r="F55" s="8"/>
       <c r="G55" s="3"/>
@@ -17418,9 +16853,9 @@
       </c>
     </row>
     <row r="56" spans="2:26" ht="15" thickBot="1">
-      <c r="B56" s="56"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="52"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="12"/>
       <c r="F56" s="13"/>
       <c r="G56" s="5"/>
@@ -17447,21 +16882,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D5:Z56" xr:uid="{8A670207-E8A0-4871-A322-7DE98FE53318}">
-    <filterColumn colId="2" showButton="0"/>
-    <filterColumn colId="4" showButton="0"/>
-    <filterColumn colId="6" showButton="0"/>
-    <filterColumn colId="8" showButton="0"/>
-    <filterColumn colId="10" showButton="0"/>
-    <filterColumn colId="12" showButton="0"/>
-    <filterColumn colId="14" showButton="0"/>
-    <filterColumn colId="16" showButton="0"/>
-    <filterColumn colId="18" showButton="0"/>
-  </autoFilter>
   <mergeCells count="34">
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="B2:X2"/>
     <mergeCell ref="C3:C5"/>
@@ -17484,15 +16905,18 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:E100 X6:X100">
     <cfRule type="expression" dxfId="11" priority="14">
@@ -17504,47 +16928,47 @@
       <formula>$F$5</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>$H$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>$J$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>$T$5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">

</xml_diff>

<commit_message>
test commit after anonymising
</commit_message>
<xml_diff>
--- a/final/leaderboard.xlsx
+++ b/final/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meInspiron\Desktop\ipl_polls\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8A8927-27B7-4979-82DA-C0CDAACC55F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E961F7-6BA7-4B6E-9EBB-AF8EC978C3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{33315BC7-FE13-4B47-AD11-5FFBB64D564A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="247">
   <si>
     <t>Username</t>
   </si>
@@ -1460,6 +1460,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1490,42 +1515,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1552,6 +1541,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1598,78 +1623,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF3FB"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2108,6 +2066,48 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBF3FB"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2462,33 +2462,33 @@
   <sheetData>
     <row r="1" spans="2:12" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:12">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="41" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="56" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2505,18 +2505,18 @@
       <c r="E3" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="44"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B4" s="97"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="30"/>
-      <c r="D4" s="97"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="30"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
@@ -2524,12 +2524,12 @@
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
-      <c r="L4" s="94"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B5" s="98"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="98"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="3"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
@@ -2537,12 +2537,12 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
-      <c r="L5" s="95"/>
+      <c r="L5" s="49"/>
     </row>
     <row r="6" spans="2:12" ht="15" customHeight="1">
-      <c r="B6" s="98"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="98"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="3"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
@@ -2550,12 +2550,12 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="95"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="98"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="98"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="3"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
@@ -2563,12 +2563,12 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="95"/>
+      <c r="L7" s="49"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="98"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="98"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="3"/>
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
@@ -2576,12 +2576,12 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="95"/>
+      <c r="L8" s="49"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="98"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="98"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="3"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
@@ -2589,12 +2589,12 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
-      <c r="L9" s="95"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="98"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="98"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="3"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -2602,12 +2602,12 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
-      <c r="L10" s="95"/>
+      <c r="L10" s="49"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="98"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="98"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="3"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
@@ -2615,12 +2615,12 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
-      <c r="L11" s="95"/>
+      <c r="L11" s="49"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="98"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="98"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="3"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
@@ -2628,12 +2628,12 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="95"/>
+      <c r="L12" s="49"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="98"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="98"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="3"/>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
@@ -2641,12 +2641,12 @@
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="95"/>
+      <c r="L13" s="49"/>
     </row>
     <row r="14" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B14" s="98"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="98"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="3"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -2654,12 +2654,12 @@
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
-      <c r="L14" s="95"/>
+      <c r="L14" s="49"/>
     </row>
     <row r="15" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B15" s="98"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="98"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="3"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
@@ -2667,12 +2667,12 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="95"/>
+      <c r="L15" s="49"/>
     </row>
     <row r="16" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B16" s="98"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="98"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="3"/>
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
@@ -2680,12 +2680,12 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="95"/>
+      <c r="L16" s="49"/>
     </row>
     <row r="17" spans="2:12" ht="14.25" customHeight="1">
-      <c r="B17" s="98"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="98"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="3"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
@@ -2693,12 +2693,12 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="95"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="98"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="98"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="3"/>
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
@@ -2706,12 +2706,12 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
-      <c r="L18" s="95"/>
+      <c r="L18" s="49"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="98"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="98"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="3"/>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
@@ -2719,12 +2719,12 @@
       <c r="I19" s="20"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
-      <c r="L19" s="95"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="98"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="98"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="3"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24"/>
@@ -2732,12 +2732,12 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
-      <c r="L20" s="95"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="98"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="98"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="3"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
@@ -2745,12 +2745,12 @@
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
-      <c r="L21" s="95"/>
+      <c r="L21" s="49"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="98"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="98"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="3"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
@@ -2758,12 +2758,12 @@
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
-      <c r="L22" s="95"/>
+      <c r="L22" s="49"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="98"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="98"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="3"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
@@ -2771,12 +2771,12 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
-      <c r="L23" s="95"/>
+      <c r="L23" s="49"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="98"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="98"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="3"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
@@ -2784,12 +2784,12 @@
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
-      <c r="L24" s="95"/>
+      <c r="L24" s="49"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="98"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="98"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="3"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
@@ -2797,12 +2797,12 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="95"/>
+      <c r="L25" s="49"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="98"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="98"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="3"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -2810,12 +2810,12 @@
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
-      <c r="L26" s="95"/>
+      <c r="L26" s="49"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="98"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="98"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="3"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
@@ -2823,12 +2823,12 @@
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
-      <c r="L27" s="95"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="98"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="98"/>
+      <c r="D28" s="52"/>
       <c r="E28" s="3"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
@@ -2836,12 +2836,12 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
-      <c r="L28" s="95"/>
+      <c r="L28" s="49"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="98"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="98"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="3"/>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
@@ -2849,12 +2849,12 @@
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
-      <c r="L29" s="95"/>
+      <c r="L29" s="49"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="98"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="98"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="3"/>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
@@ -2862,12 +2862,12 @@
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
-      <c r="L30" s="95"/>
+      <c r="L30" s="49"/>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="98"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="98"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="3"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
@@ -2875,12 +2875,12 @@
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
-      <c r="L31" s="95"/>
+      <c r="L31" s="49"/>
     </row>
     <row r="32" spans="2:12">
-      <c r="B32" s="98"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="98"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="3"/>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
@@ -2888,12 +2888,12 @@
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
-      <c r="L32" s="95"/>
+      <c r="L32" s="49"/>
     </row>
     <row r="33" spans="2:12">
-      <c r="B33" s="98"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="98"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="3"/>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
@@ -2901,12 +2901,12 @@
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
       <c r="K33" s="20"/>
-      <c r="L33" s="95"/>
+      <c r="L33" s="49"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="98"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="98"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="3"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
@@ -2914,12 +2914,12 @@
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
-      <c r="L34" s="95"/>
+      <c r="L34" s="49"/>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="98"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="98"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="3"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
@@ -2927,12 +2927,12 @@
       <c r="I35" s="20"/>
       <c r="J35" s="20"/>
       <c r="K35" s="20"/>
-      <c r="L35" s="95"/>
+      <c r="L35" s="49"/>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="98"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="98"/>
+      <c r="D36" s="52"/>
       <c r="E36" s="3"/>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
@@ -2940,12 +2940,12 @@
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="95"/>
+      <c r="L36" s="49"/>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="98"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="98"/>
+      <c r="D37" s="52"/>
       <c r="E37" s="3"/>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
@@ -2953,12 +2953,12 @@
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
-      <c r="L37" s="95"/>
+      <c r="L37" s="49"/>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="98"/>
+      <c r="B38" s="52"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="98"/>
+      <c r="D38" s="52"/>
       <c r="E38" s="3"/>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
@@ -2966,12 +2966,12 @@
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
-      <c r="L38" s="95"/>
+      <c r="L38" s="49"/>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="98"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="98"/>
+      <c r="D39" s="52"/>
       <c r="E39" s="3"/>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
@@ -2979,12 +2979,12 @@
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
       <c r="K39" s="20"/>
-      <c r="L39" s="95"/>
+      <c r="L39" s="49"/>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="98"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="98"/>
+      <c r="D40" s="52"/>
       <c r="E40" s="3"/>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
@@ -2992,12 +2992,12 @@
       <c r="I40" s="20"/>
       <c r="J40" s="20"/>
       <c r="K40" s="20"/>
-      <c r="L40" s="95"/>
+      <c r="L40" s="49"/>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="98"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="98"/>
+      <c r="D41" s="52"/>
       <c r="E41" s="3"/>
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
@@ -3005,12 +3005,12 @@
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="95"/>
+      <c r="L41" s="49"/>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="98"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="98"/>
+      <c r="D42" s="52"/>
       <c r="E42" s="3"/>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
@@ -3018,12 +3018,12 @@
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
-      <c r="L42" s="95"/>
+      <c r="L42" s="49"/>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="98"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="98"/>
+      <c r="D43" s="52"/>
       <c r="E43" s="3"/>
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
@@ -3031,12 +3031,12 @@
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
-      <c r="L43" s="95"/>
+      <c r="L43" s="49"/>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="98"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="98"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="3"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
@@ -3044,12 +3044,12 @@
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="95"/>
+      <c r="L44" s="49"/>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="98"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="98"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="3"/>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
@@ -3057,12 +3057,12 @@
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
-      <c r="L45" s="95"/>
+      <c r="L45" s="49"/>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="98"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="98"/>
+      <c r="D46" s="52"/>
       <c r="E46" s="3"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
@@ -3070,12 +3070,12 @@
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
       <c r="K46" s="20"/>
-      <c r="L46" s="95"/>
+      <c r="L46" s="49"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="98"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="98"/>
+      <c r="D47" s="52"/>
       <c r="E47" s="3"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
@@ -3083,12 +3083,12 @@
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
       <c r="K47" s="20"/>
-      <c r="L47" s="95"/>
+      <c r="L47" s="49"/>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="98"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="98"/>
+      <c r="D48" s="52"/>
       <c r="E48" s="3"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
@@ -3096,12 +3096,12 @@
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
       <c r="K48" s="20"/>
-      <c r="L48" s="95"/>
+      <c r="L48" s="49"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="98"/>
+      <c r="B49" s="52"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="98"/>
+      <c r="D49" s="52"/>
       <c r="E49" s="3"/>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
@@ -3109,12 +3109,12 @@
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
       <c r="K49" s="20"/>
-      <c r="L49" s="95"/>
+      <c r="L49" s="49"/>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="98"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="98"/>
+      <c r="D50" s="52"/>
       <c r="E50" s="3"/>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
@@ -3122,12 +3122,12 @@
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
       <c r="K50" s="20"/>
-      <c r="L50" s="95"/>
+      <c r="L50" s="49"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="98"/>
+      <c r="B51" s="52"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="98"/>
+      <c r="D51" s="52"/>
       <c r="E51" s="3"/>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
@@ -3135,12 +3135,12 @@
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
-      <c r="L51" s="95"/>
+      <c r="L51" s="49"/>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="98"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="98"/>
+      <c r="D52" s="52"/>
       <c r="E52" s="3"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
@@ -3148,12 +3148,12 @@
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
-      <c r="L52" s="95"/>
+      <c r="L52" s="49"/>
     </row>
     <row r="53" spans="2:12">
-      <c r="B53" s="98"/>
+      <c r="B53" s="52"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="98"/>
+      <c r="D53" s="52"/>
       <c r="E53" s="3"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
@@ -3161,12 +3161,12 @@
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
-      <c r="L53" s="95"/>
+      <c r="L53" s="49"/>
     </row>
     <row r="54" spans="2:12">
-      <c r="B54" s="98"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="98"/>
+      <c r="D54" s="52"/>
       <c r="E54" s="3"/>
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
@@ -3174,12 +3174,12 @@
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
       <c r="K54" s="20"/>
-      <c r="L54" s="95"/>
+      <c r="L54" s="49"/>
     </row>
     <row r="55" spans="2:12">
-      <c r="B55" s="98"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="98"/>
+      <c r="D55" s="52"/>
       <c r="E55" s="3"/>
       <c r="F55" s="24"/>
       <c r="G55" s="24"/>
@@ -3187,12 +3187,12 @@
       <c r="I55" s="20"/>
       <c r="J55" s="20"/>
       <c r="K55" s="20"/>
-      <c r="L55" s="95"/>
+      <c r="L55" s="49"/>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="98"/>
+      <c r="B56" s="52"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="98"/>
+      <c r="D56" s="52"/>
       <c r="E56" s="3"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
@@ -3200,12 +3200,12 @@
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
       <c r="K56" s="20"/>
-      <c r="L56" s="95"/>
+      <c r="L56" s="49"/>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="98"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="98"/>
+      <c r="D57" s="52"/>
       <c r="E57" s="3"/>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
@@ -3213,12 +3213,12 @@
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
-      <c r="L57" s="95"/>
+      <c r="L57" s="49"/>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="98"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="98"/>
+      <c r="D58" s="52"/>
       <c r="E58" s="3"/>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
@@ -3226,12 +3226,12 @@
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
       <c r="K58" s="20"/>
-      <c r="L58" s="95"/>
+      <c r="L58" s="49"/>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="98"/>
+      <c r="B59" s="52"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="98"/>
+      <c r="D59" s="52"/>
       <c r="E59" s="3"/>
       <c r="F59" s="24"/>
       <c r="G59" s="24"/>
@@ -3239,12 +3239,12 @@
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
-      <c r="L59" s="95"/>
+      <c r="L59" s="49"/>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="98"/>
+      <c r="B60" s="52"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="98"/>
+      <c r="D60" s="52"/>
       <c r="E60" s="3"/>
       <c r="F60" s="24"/>
       <c r="G60" s="24"/>
@@ -3252,12 +3252,12 @@
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
       <c r="K60" s="20"/>
-      <c r="L60" s="95"/>
+      <c r="L60" s="49"/>
     </row>
     <row r="61" spans="2:12">
-      <c r="B61" s="98"/>
+      <c r="B61" s="52"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="98"/>
+      <c r="D61" s="52"/>
       <c r="E61" s="3"/>
       <c r="F61" s="24"/>
       <c r="G61" s="24"/>
@@ -3265,12 +3265,12 @@
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
       <c r="K61" s="20"/>
-      <c r="L61" s="95"/>
+      <c r="L61" s="49"/>
     </row>
     <row r="62" spans="2:12">
-      <c r="B62" s="98"/>
+      <c r="B62" s="52"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="98"/>
+      <c r="D62" s="52"/>
       <c r="E62" s="3"/>
       <c r="F62" s="24"/>
       <c r="G62" s="24"/>
@@ -3278,12 +3278,12 @@
       <c r="I62" s="20"/>
       <c r="J62" s="20"/>
       <c r="K62" s="20"/>
-      <c r="L62" s="95"/>
+      <c r="L62" s="49"/>
     </row>
     <row r="63" spans="2:12">
-      <c r="B63" s="98"/>
+      <c r="B63" s="52"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="98"/>
+      <c r="D63" s="52"/>
       <c r="E63" s="3"/>
       <c r="F63" s="24"/>
       <c r="G63" s="24"/>
@@ -3291,12 +3291,12 @@
       <c r="I63" s="20"/>
       <c r="J63" s="20"/>
       <c r="K63" s="20"/>
-      <c r="L63" s="95"/>
+      <c r="L63" s="49"/>
     </row>
     <row r="64" spans="2:12">
-      <c r="B64" s="98"/>
+      <c r="B64" s="52"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="98"/>
+      <c r="D64" s="52"/>
       <c r="E64" s="3"/>
       <c r="F64" s="24"/>
       <c r="G64" s="24"/>
@@ -3304,12 +3304,12 @@
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
       <c r="K64" s="20"/>
-      <c r="L64" s="95"/>
+      <c r="L64" s="49"/>
     </row>
     <row r="65" spans="2:12">
-      <c r="B65" s="98"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="98"/>
+      <c r="D65" s="52"/>
       <c r="E65" s="3"/>
       <c r="F65" s="24"/>
       <c r="G65" s="24"/>
@@ -3317,12 +3317,12 @@
       <c r="I65" s="20"/>
       <c r="J65" s="20"/>
       <c r="K65" s="20"/>
-      <c r="L65" s="95"/>
+      <c r="L65" s="49"/>
     </row>
     <row r="66" spans="2:12">
-      <c r="B66" s="98"/>
+      <c r="B66" s="52"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="98"/>
+      <c r="D66" s="52"/>
       <c r="E66" s="3"/>
       <c r="F66" s="24"/>
       <c r="G66" s="24"/>
@@ -3330,12 +3330,12 @@
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
       <c r="K66" s="20"/>
-      <c r="L66" s="95"/>
+      <c r="L66" s="49"/>
     </row>
     <row r="67" spans="2:12">
-      <c r="B67" s="98"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="98"/>
+      <c r="D67" s="52"/>
       <c r="E67" s="3"/>
       <c r="F67" s="24"/>
       <c r="G67" s="24"/>
@@ -3343,12 +3343,12 @@
       <c r="I67" s="20"/>
       <c r="J67" s="20"/>
       <c r="K67" s="20"/>
-      <c r="L67" s="95"/>
+      <c r="L67" s="49"/>
     </row>
     <row r="68" spans="2:12">
-      <c r="B68" s="98"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="98"/>
+      <c r="D68" s="52"/>
       <c r="E68" s="3"/>
       <c r="F68" s="24"/>
       <c r="G68" s="24"/>
@@ -3356,12 +3356,12 @@
       <c r="I68" s="20"/>
       <c r="J68" s="20"/>
       <c r="K68" s="20"/>
-      <c r="L68" s="95"/>
+      <c r="L68" s="49"/>
     </row>
     <row r="69" spans="2:12">
-      <c r="B69" s="98"/>
+      <c r="B69" s="52"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="98"/>
+      <c r="D69" s="52"/>
       <c r="E69" s="3"/>
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
@@ -3369,12 +3369,12 @@
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
-      <c r="L69" s="95"/>
+      <c r="L69" s="49"/>
     </row>
     <row r="70" spans="2:12">
-      <c r="B70" s="98"/>
+      <c r="B70" s="52"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="98"/>
+      <c r="D70" s="52"/>
       <c r="E70" s="3"/>
       <c r="F70" s="24"/>
       <c r="G70" s="24"/>
@@ -3382,12 +3382,12 @@
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
-      <c r="L70" s="95"/>
+      <c r="L70" s="49"/>
     </row>
     <row r="71" spans="2:12">
-      <c r="B71" s="98"/>
+      <c r="B71" s="52"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="98"/>
+      <c r="D71" s="52"/>
       <c r="E71" s="3"/>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
@@ -3395,12 +3395,12 @@
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
       <c r="K71" s="20"/>
-      <c r="L71" s="95"/>
+      <c r="L71" s="49"/>
     </row>
     <row r="72" spans="2:12">
-      <c r="B72" s="98"/>
+      <c r="B72" s="52"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="98"/>
+      <c r="D72" s="52"/>
       <c r="E72" s="3"/>
       <c r="F72" s="24"/>
       <c r="G72" s="24"/>
@@ -3408,12 +3408,12 @@
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
       <c r="K72" s="20"/>
-      <c r="L72" s="95"/>
+      <c r="L72" s="49"/>
     </row>
     <row r="73" spans="2:12">
-      <c r="B73" s="98"/>
+      <c r="B73" s="52"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="98"/>
+      <c r="D73" s="52"/>
       <c r="E73" s="3"/>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
@@ -3421,12 +3421,12 @@
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
       <c r="K73" s="20"/>
-      <c r="L73" s="95"/>
+      <c r="L73" s="49"/>
     </row>
     <row r="74" spans="2:12">
-      <c r="B74" s="98"/>
+      <c r="B74" s="52"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="98"/>
+      <c r="D74" s="52"/>
       <c r="E74" s="3"/>
       <c r="F74" s="24"/>
       <c r="G74" s="24"/>
@@ -3434,12 +3434,12 @@
       <c r="I74" s="20"/>
       <c r="J74" s="20"/>
       <c r="K74" s="20"/>
-      <c r="L74" s="95"/>
+      <c r="L74" s="49"/>
     </row>
     <row r="75" spans="2:12">
-      <c r="B75" s="98"/>
+      <c r="B75" s="52"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="98"/>
+      <c r="D75" s="52"/>
       <c r="E75" s="3"/>
       <c r="F75" s="24"/>
       <c r="G75" s="24"/>
@@ -3447,12 +3447,12 @@
       <c r="I75" s="20"/>
       <c r="J75" s="20"/>
       <c r="K75" s="20"/>
-      <c r="L75" s="95"/>
+      <c r="L75" s="49"/>
     </row>
     <row r="76" spans="2:12">
-      <c r="B76" s="98"/>
+      <c r="B76" s="52"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="98"/>
+      <c r="D76" s="52"/>
       <c r="E76" s="3"/>
       <c r="F76" s="24"/>
       <c r="G76" s="24"/>
@@ -3460,12 +3460,12 @@
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
       <c r="K76" s="20"/>
-      <c r="L76" s="95"/>
+      <c r="L76" s="49"/>
     </row>
     <row r="77" spans="2:12">
-      <c r="B77" s="98"/>
+      <c r="B77" s="52"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="98"/>
+      <c r="D77" s="52"/>
       <c r="E77" s="3"/>
       <c r="F77" s="24"/>
       <c r="G77" s="24"/>
@@ -3473,12 +3473,12 @@
       <c r="I77" s="20"/>
       <c r="J77" s="20"/>
       <c r="K77" s="20"/>
-      <c r="L77" s="95"/>
+      <c r="L77" s="49"/>
     </row>
     <row r="78" spans="2:12">
-      <c r="B78" s="98"/>
+      <c r="B78" s="52"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="98"/>
+      <c r="D78" s="52"/>
       <c r="E78" s="3"/>
       <c r="F78" s="24"/>
       <c r="G78" s="24"/>
@@ -3486,12 +3486,12 @@
       <c r="I78" s="20"/>
       <c r="J78" s="20"/>
       <c r="K78" s="20"/>
-      <c r="L78" s="95"/>
+      <c r="L78" s="49"/>
     </row>
     <row r="79" spans="2:12">
-      <c r="B79" s="98"/>
+      <c r="B79" s="52"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="98"/>
+      <c r="D79" s="52"/>
       <c r="E79" s="3"/>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
@@ -3499,12 +3499,12 @@
       <c r="I79" s="20"/>
       <c r="J79" s="20"/>
       <c r="K79" s="20"/>
-      <c r="L79" s="95"/>
+      <c r="L79" s="49"/>
     </row>
     <row r="80" spans="2:12">
-      <c r="B80" s="98"/>
+      <c r="B80" s="52"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="98"/>
+      <c r="D80" s="52"/>
       <c r="E80" s="3"/>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
@@ -3512,12 +3512,12 @@
       <c r="I80" s="20"/>
       <c r="J80" s="20"/>
       <c r="K80" s="20"/>
-      <c r="L80" s="95"/>
+      <c r="L80" s="49"/>
     </row>
     <row r="81" spans="2:12">
-      <c r="B81" s="98"/>
+      <c r="B81" s="52"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="98"/>
+      <c r="D81" s="52"/>
       <c r="E81" s="3"/>
       <c r="F81" s="24"/>
       <c r="G81" s="24"/>
@@ -3525,12 +3525,12 @@
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
       <c r="K81" s="20"/>
-      <c r="L81" s="95"/>
+      <c r="L81" s="49"/>
     </row>
     <row r="82" spans="2:12">
-      <c r="B82" s="98"/>
+      <c r="B82" s="52"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="98"/>
+      <c r="D82" s="52"/>
       <c r="E82" s="3"/>
       <c r="F82" s="24"/>
       <c r="G82" s="24"/>
@@ -3538,12 +3538,12 @@
       <c r="I82" s="20"/>
       <c r="J82" s="20"/>
       <c r="K82" s="20"/>
-      <c r="L82" s="95"/>
+      <c r="L82" s="49"/>
     </row>
     <row r="83" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B83" s="99"/>
+      <c r="B83" s="53"/>
       <c r="C83" s="5"/>
-      <c r="D83" s="99"/>
+      <c r="D83" s="53"/>
       <c r="E83" s="5"/>
       <c r="F83" s="25"/>
       <c r="G83" s="25"/>
@@ -3551,7 +3551,7 @@
       <c r="I83" s="21"/>
       <c r="J83" s="21"/>
       <c r="K83" s="21"/>
-      <c r="L83" s="96"/>
+      <c r="L83" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3566,21 +3566,21 @@
     <mergeCell ref="I2:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:L150">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="49" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C150 E4:E150">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="48" priority="2" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="—">
+    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="—">
       <formula>NOT(ISERROR(SEARCH("—",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="↓">
+    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="45" priority="5" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3602,7 +3602,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0.625" customWidth="1"/>
-    <col min="2" max="3" width="11.375" style="87" customWidth="1"/>
+    <col min="2" max="3" width="11.375" style="41" customWidth="1"/>
     <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.625" style="1" customWidth="1"/>
@@ -3629,169 +3629,171 @@
   <sheetData>
     <row r="1" spans="2:26" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="66"/>
     </row>
     <row r="3" spans="2:26" ht="15" customHeight="1">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="70" t="s">
         <v>243</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="45" t="s">
+      <c r="D3" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="45" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="45" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>226</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
+      <c r="Q3" s="59"/>
+      <c r="R3" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="45" t="s">
+      <c r="S3" s="59"/>
+      <c r="T3" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="45" t="s">
+      <c r="U3" s="59"/>
+      <c r="V3" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="W3" s="46"/>
-      <c r="X3" s="66" t="s">
+      <c r="W3" s="59"/>
+      <c r="X3" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="57" t="s">
+      <c r="Z3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26">
-      <c r="B4" s="70"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="59" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="73" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="59" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="59" t="s">
+      <c r="K4" s="74"/>
+      <c r="L4" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="59" t="s">
+      <c r="M4" s="74"/>
+      <c r="N4" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="59" t="s">
+      <c r="O4" s="74"/>
+      <c r="P4" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="59" t="s">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="73" t="s">
         <v>238</v>
       </c>
-      <c r="S4" s="60"/>
-      <c r="T4" s="59" t="s">
+      <c r="S4" s="74"/>
+      <c r="T4" s="73" t="s">
         <v>239</v>
       </c>
-      <c r="U4" s="60"/>
-      <c r="V4" s="59" t="s">
+      <c r="U4" s="74"/>
+      <c r="V4" s="73" t="s">
         <v>240</v>
       </c>
-      <c r="W4" s="60"/>
-      <c r="X4" s="67"/>
-      <c r="Z4" s="58"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="68"/>
+      <c r="Z4" s="78"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B5" s="71"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="61" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="62"/>
-      <c r="H5" s="61" t="s">
+      <c r="G5" s="76"/>
+      <c r="H5" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="62"/>
-      <c r="J5" s="61" t="s">
+      <c r="I5" s="76"/>
+      <c r="J5" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="61" t="s">
+      <c r="K5" s="76"/>
+      <c r="L5" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="62"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="61"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="62"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="62"/>
-      <c r="X5" s="68"/>
-      <c r="Z5" s="58"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="O5" s="76"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="76"/>
+      <c r="X5" s="69"/>
+      <c r="Z5" s="78"/>
     </row>
     <row r="6" spans="2:26">
-      <c r="B6" s="88"/>
-      <c r="C6" s="91"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
@@ -3819,8 +3821,8 @@
       </c>
     </row>
     <row r="7" spans="2:26">
-      <c r="B7" s="89"/>
-      <c r="C7" s="92"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="22"/>
       <c r="E7" s="11"/>
       <c r="F7" s="8"/>
@@ -3848,8 +3850,8 @@
       </c>
     </row>
     <row r="8" spans="2:26">
-      <c r="B8" s="89"/>
-      <c r="C8" s="92"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="22"/>
       <c r="E8" s="11"/>
       <c r="F8" s="2"/>
@@ -3877,8 +3879,8 @@
       </c>
     </row>
     <row r="9" spans="2:26">
-      <c r="B9" s="89"/>
-      <c r="C9" s="92"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="22"/>
       <c r="E9" s="11"/>
       <c r="F9" s="8"/>
@@ -3906,8 +3908,8 @@
       </c>
     </row>
     <row r="10" spans="2:26">
-      <c r="B10" s="89"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="22"/>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
@@ -3935,8 +3937,8 @@
       </c>
     </row>
     <row r="11" spans="2:26">
-      <c r="B11" s="89"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="22"/>
       <c r="E11" s="11"/>
       <c r="F11" s="2"/>
@@ -3964,8 +3966,8 @@
       </c>
     </row>
     <row r="12" spans="2:26">
-      <c r="B12" s="89"/>
-      <c r="C12" s="92"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="22"/>
       <c r="E12" s="11"/>
       <c r="F12" s="2"/>
@@ -3993,8 +3995,8 @@
       </c>
     </row>
     <row r="13" spans="2:26">
-      <c r="B13" s="89"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="22"/>
       <c r="E13" s="11"/>
       <c r="F13" s="2"/>
@@ -4022,8 +4024,8 @@
       </c>
     </row>
     <row r="14" spans="2:26">
-      <c r="B14" s="89"/>
-      <c r="C14" s="92"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="22"/>
       <c r="E14" s="11"/>
       <c r="F14" s="8"/>
@@ -4051,8 +4053,8 @@
       </c>
     </row>
     <row r="15" spans="2:26">
-      <c r="B15" s="89"/>
-      <c r="C15" s="92"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="22"/>
       <c r="E15" s="11"/>
       <c r="F15" s="8"/>
@@ -4080,8 +4082,8 @@
       </c>
     </row>
     <row r="16" spans="2:26">
-      <c r="B16" s="89"/>
-      <c r="C16" s="92"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="22"/>
       <c r="E16" s="11"/>
       <c r="F16" s="8"/>
@@ -4109,8 +4111,8 @@
       </c>
     </row>
     <row r="17" spans="2:26">
-      <c r="B17" s="89"/>
-      <c r="C17" s="92"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="22"/>
       <c r="E17" s="11"/>
       <c r="F17" s="8"/>
@@ -4138,8 +4140,8 @@
       </c>
     </row>
     <row r="18" spans="2:26">
-      <c r="B18" s="89"/>
-      <c r="C18" s="92"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="22"/>
       <c r="E18" s="11"/>
       <c r="F18" s="8"/>
@@ -4167,8 +4169,8 @@
       </c>
     </row>
     <row r="19" spans="2:26">
-      <c r="B19" s="89"/>
-      <c r="C19" s="92"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="22"/>
       <c r="E19" s="11"/>
       <c r="F19" s="2"/>
@@ -4196,8 +4198,8 @@
       </c>
     </row>
     <row r="20" spans="2:26">
-      <c r="B20" s="89"/>
-      <c r="C20" s="92"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="22"/>
       <c r="E20" s="11"/>
       <c r="F20" s="2"/>
@@ -4225,8 +4227,8 @@
       </c>
     </row>
     <row r="21" spans="2:26">
-      <c r="B21" s="89"/>
-      <c r="C21" s="92"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="22"/>
       <c r="E21" s="11"/>
       <c r="F21" s="8"/>
@@ -4254,8 +4256,8 @@
       </c>
     </row>
     <row r="22" spans="2:26">
-      <c r="B22" s="89"/>
-      <c r="C22" s="92"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="22"/>
       <c r="E22" s="11"/>
       <c r="F22" s="8"/>
@@ -4283,8 +4285,8 @@
       </c>
     </row>
     <row r="23" spans="2:26">
-      <c r="B23" s="89"/>
-      <c r="C23" s="92"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="22"/>
       <c r="E23" s="11"/>
       <c r="F23" s="8"/>
@@ -4312,8 +4314,8 @@
       </c>
     </row>
     <row r="24" spans="2:26">
-      <c r="B24" s="89"/>
-      <c r="C24" s="92"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="22"/>
       <c r="E24" s="11"/>
       <c r="F24" s="8"/>
@@ -4341,8 +4343,8 @@
       </c>
     </row>
     <row r="25" spans="2:26">
-      <c r="B25" s="89"/>
-      <c r="C25" s="92"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="22"/>
       <c r="E25" s="11"/>
       <c r="F25" s="8"/>
@@ -4370,8 +4372,8 @@
       </c>
     </row>
     <row r="26" spans="2:26">
-      <c r="B26" s="89"/>
-      <c r="C26" s="92"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="22"/>
       <c r="E26" s="11"/>
       <c r="F26" s="8"/>
@@ -4399,8 +4401,8 @@
       </c>
     </row>
     <row r="27" spans="2:26">
-      <c r="B27" s="89"/>
-      <c r="C27" s="92"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="22"/>
       <c r="E27" s="11"/>
       <c r="F27" s="8"/>
@@ -4428,8 +4430,8 @@
       </c>
     </row>
     <row r="28" spans="2:26">
-      <c r="B28" s="89"/>
-      <c r="C28" s="92"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="22"/>
       <c r="E28" s="11"/>
       <c r="F28" s="8"/>
@@ -4457,8 +4459,8 @@
       </c>
     </row>
     <row r="29" spans="2:26">
-      <c r="B29" s="89"/>
-      <c r="C29" s="92"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="22"/>
       <c r="E29" s="11"/>
       <c r="F29" s="8"/>
@@ -4486,8 +4488,8 @@
       </c>
     </row>
     <row r="30" spans="2:26">
-      <c r="B30" s="89"/>
-      <c r="C30" s="92"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="22"/>
       <c r="E30" s="11"/>
       <c r="F30" s="2"/>
@@ -4515,8 +4517,8 @@
       </c>
     </row>
     <row r="31" spans="2:26">
-      <c r="B31" s="89"/>
-      <c r="C31" s="92"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="22"/>
       <c r="E31" s="11"/>
       <c r="F31" s="2"/>
@@ -4544,8 +4546,8 @@
       </c>
     </row>
     <row r="32" spans="2:26">
-      <c r="B32" s="89"/>
-      <c r="C32" s="92"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="22"/>
       <c r="E32" s="11"/>
       <c r="F32" s="2"/>
@@ -4573,8 +4575,8 @@
       </c>
     </row>
     <row r="33" spans="2:26">
-      <c r="B33" s="89"/>
-      <c r="C33" s="92"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="46"/>
       <c r="D33" s="22"/>
       <c r="E33" s="11"/>
       <c r="F33" s="8"/>
@@ -4602,8 +4604,8 @@
       </c>
     </row>
     <row r="34" spans="2:26">
-      <c r="B34" s="89"/>
-      <c r="C34" s="92"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="22"/>
       <c r="E34" s="11"/>
       <c r="F34" s="8"/>
@@ -4631,8 +4633,8 @@
       </c>
     </row>
     <row r="35" spans="2:26">
-      <c r="B35" s="89"/>
-      <c r="C35" s="92"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="22"/>
       <c r="E35" s="11"/>
       <c r="F35" s="8"/>
@@ -4660,8 +4662,8 @@
       </c>
     </row>
     <row r="36" spans="2:26">
-      <c r="B36" s="89"/>
-      <c r="C36" s="92"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="22"/>
       <c r="E36" s="11"/>
       <c r="F36" s="8"/>
@@ -4689,8 +4691,8 @@
       </c>
     </row>
     <row r="37" spans="2:26">
-      <c r="B37" s="89"/>
-      <c r="C37" s="92"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="22"/>
       <c r="E37" s="11"/>
       <c r="F37" s="8"/>
@@ -4718,8 +4720,8 @@
       </c>
     </row>
     <row r="38" spans="2:26">
-      <c r="B38" s="89"/>
-      <c r="C38" s="92"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="22"/>
       <c r="E38" s="11"/>
       <c r="F38" s="8"/>
@@ -4747,8 +4749,8 @@
       </c>
     </row>
     <row r="39" spans="2:26">
-      <c r="B39" s="89"/>
-      <c r="C39" s="92"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="46"/>
       <c r="D39" s="22"/>
       <c r="E39" s="11"/>
       <c r="F39" s="8"/>
@@ -4776,8 +4778,8 @@
       </c>
     </row>
     <row r="40" spans="2:26">
-      <c r="B40" s="89"/>
-      <c r="C40" s="92"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="46"/>
       <c r="D40" s="22"/>
       <c r="E40" s="11"/>
       <c r="F40" s="8"/>
@@ -4805,8 +4807,8 @@
       </c>
     </row>
     <row r="41" spans="2:26">
-      <c r="B41" s="89"/>
-      <c r="C41" s="92"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="46"/>
       <c r="D41" s="22"/>
       <c r="E41" s="11"/>
       <c r="F41" s="8"/>
@@ -4834,8 +4836,8 @@
       </c>
     </row>
     <row r="42" spans="2:26">
-      <c r="B42" s="89"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="46"/>
       <c r="D42" s="22"/>
       <c r="E42" s="11"/>
       <c r="F42" s="8"/>
@@ -4863,8 +4865,8 @@
       </c>
     </row>
     <row r="43" spans="2:26">
-      <c r="B43" s="89"/>
-      <c r="C43" s="92"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="46"/>
       <c r="D43" s="22"/>
       <c r="E43" s="11"/>
       <c r="F43" s="8"/>
@@ -4892,8 +4894,8 @@
       </c>
     </row>
     <row r="44" spans="2:26">
-      <c r="B44" s="89"/>
-      <c r="C44" s="92"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="46"/>
       <c r="D44" s="22"/>
       <c r="E44" s="11"/>
       <c r="F44" s="8"/>
@@ -4921,8 +4923,8 @@
       </c>
     </row>
     <row r="45" spans="2:26">
-      <c r="B45" s="89"/>
-      <c r="C45" s="92"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="46"/>
       <c r="D45" s="22"/>
       <c r="E45" s="11"/>
       <c r="F45" s="8"/>
@@ -4950,8 +4952,8 @@
       </c>
     </row>
     <row r="46" spans="2:26">
-      <c r="B46" s="89"/>
-      <c r="C46" s="92"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="22"/>
       <c r="E46" s="11"/>
       <c r="F46" s="8"/>
@@ -4979,8 +4981,8 @@
       </c>
     </row>
     <row r="47" spans="2:26">
-      <c r="B47" s="89"/>
-      <c r="C47" s="92"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="22"/>
       <c r="E47" s="11"/>
       <c r="F47" s="8"/>
@@ -5008,8 +5010,8 @@
       </c>
     </row>
     <row r="48" spans="2:26">
-      <c r="B48" s="89"/>
-      <c r="C48" s="92"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="46"/>
       <c r="D48" s="22"/>
       <c r="E48" s="11"/>
       <c r="F48" s="8"/>
@@ -5037,8 +5039,8 @@
       </c>
     </row>
     <row r="49" spans="2:26">
-      <c r="B49" s="89"/>
-      <c r="C49" s="92"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="46"/>
       <c r="D49" s="22"/>
       <c r="E49" s="11"/>
       <c r="F49" s="8"/>
@@ -5066,8 +5068,8 @@
       </c>
     </row>
     <row r="50" spans="2:26">
-      <c r="B50" s="89"/>
-      <c r="C50" s="92"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="22"/>
       <c r="E50" s="11"/>
       <c r="F50" s="8"/>
@@ -5095,8 +5097,8 @@
       </c>
     </row>
     <row r="51" spans="2:26">
-      <c r="B51" s="89"/>
-      <c r="C51" s="92"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="46"/>
       <c r="D51" s="22"/>
       <c r="E51" s="11"/>
       <c r="F51" s="8"/>
@@ -5124,8 +5126,8 @@
       </c>
     </row>
     <row r="52" spans="2:26">
-      <c r="B52" s="89"/>
-      <c r="C52" s="92"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="46"/>
       <c r="D52" s="22"/>
       <c r="E52" s="11"/>
       <c r="F52" s="8"/>
@@ -5153,8 +5155,8 @@
       </c>
     </row>
     <row r="53" spans="2:26">
-      <c r="B53" s="89"/>
-      <c r="C53" s="92"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="46"/>
       <c r="D53" s="22"/>
       <c r="E53" s="11"/>
       <c r="F53" s="8"/>
@@ -5182,8 +5184,8 @@
       </c>
     </row>
     <row r="54" spans="2:26">
-      <c r="B54" s="89"/>
-      <c r="C54" s="92"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="46"/>
       <c r="D54" s="22"/>
       <c r="E54" s="11"/>
       <c r="F54" s="8"/>
@@ -5211,8 +5213,8 @@
       </c>
     </row>
     <row r="55" spans="2:26">
-      <c r="B55" s="89"/>
-      <c r="C55" s="92"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="46"/>
       <c r="D55" s="22"/>
       <c r="E55" s="11"/>
       <c r="F55" s="8"/>
@@ -5240,8 +5242,8 @@
       </c>
     </row>
     <row r="56" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B56" s="90"/>
-      <c r="C56" s="93"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="47"/>
       <c r="D56" s="23"/>
       <c r="E56" s="12"/>
       <c r="F56" s="13"/>
@@ -5270,6 +5272,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
     <mergeCell ref="B2:X2"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B5"/>
@@ -5285,81 +5305,63 @@
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:X5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:E100 X6:X100">
-    <cfRule type="expression" dxfId="49" priority="14">
+    <cfRule type="expression" dxfId="44" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
       <formula>$F$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>$H$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>$J$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>$T$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>$V$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5409,177 +5411,177 @@
   <sheetData>
     <row r="1" spans="2:26" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="87" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="76"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89"/>
     </row>
     <row r="3" spans="2:26" ht="15" customHeight="1">
-      <c r="B3" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="45" t="s">
+      <c r="B3" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="45" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>193</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="45" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
+      <c r="Q3" s="59"/>
+      <c r="R3" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="45" t="s">
+      <c r="S3" s="59"/>
+      <c r="T3" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="45" t="s">
+      <c r="U3" s="59"/>
+      <c r="V3" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="W3" s="46"/>
-      <c r="X3" s="77" t="s">
+      <c r="W3" s="59"/>
+      <c r="X3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="57" t="s">
+      <c r="Z3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="15">
-      <c r="B4" s="79"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="59" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="74"/>
+      <c r="F4" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="59" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="59" t="s">
+      <c r="K4" s="74"/>
+      <c r="L4" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="59" t="s">
+      <c r="M4" s="74"/>
+      <c r="N4" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="59" t="s">
+      <c r="O4" s="74"/>
+      <c r="P4" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="59" t="s">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="73" t="s">
         <v>207</v>
       </c>
-      <c r="S4" s="60"/>
-      <c r="T4" s="59" t="s">
+      <c r="S4" s="74"/>
+      <c r="T4" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="U4" s="60"/>
-      <c r="V4" s="59" t="s">
+      <c r="U4" s="74"/>
+      <c r="V4" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="60"/>
-      <c r="X4" s="67"/>
-      <c r="Z4" s="58"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="68"/>
+      <c r="Z4" s="78"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="72" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="72" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="72" t="s">
+      <c r="G5" s="86"/>
+      <c r="H5" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="72" t="s">
+      <c r="I5" s="86"/>
+      <c r="J5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="73"/>
-      <c r="L5" s="72" t="s">
+      <c r="K5" s="86"/>
+      <c r="L5" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="72" t="s">
+      <c r="M5" s="86"/>
+      <c r="N5" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="73"/>
-      <c r="P5" s="72" t="s">
+      <c r="O5" s="86"/>
+      <c r="P5" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="72" t="s">
+      <c r="Q5" s="86"/>
+      <c r="R5" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="73"/>
-      <c r="T5" s="72" t="s">
+      <c r="S5" s="86"/>
+      <c r="T5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="U5" s="73"/>
-      <c r="V5" s="72" t="s">
+      <c r="U5" s="86"/>
+      <c r="V5" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="W5" s="73"/>
-      <c r="X5" s="68"/>
-      <c r="Z5" s="58"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="69"/>
+      <c r="Z5" s="78"/>
     </row>
     <row r="6" spans="2:26">
       <c r="B6" s="14" t="s">
@@ -9400,6 +9402,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
@@ -9416,86 +9437,67 @@
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C194 X6:X194">
-    <cfRule type="expression" dxfId="37" priority="46">
+    <cfRule type="expression" dxfId="32" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
       <formula>$D$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576 U1:U1048576 W1:W1048576">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="44" operator="equal">
       <formula>$F$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
       <formula>$H$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="31" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="42" operator="equal">
       <formula>$J$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="40" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="39" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="27" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T1048576">
-    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="37" operator="equal">
       <formula>$T$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
       <formula>$V$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9541,149 +9543,149 @@
   <sheetData>
     <row r="1" spans="2:22" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="76"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="89"/>
     </row>
     <row r="3" spans="2:22" ht="15" customHeight="1">
-      <c r="B3" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="45" t="s">
+      <c r="B3" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="45" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="45" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45" t="s">
+      <c r="Q3" s="59"/>
+      <c r="R3" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="77" t="s">
+      <c r="S3" s="59"/>
+      <c r="T3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="57" t="s">
+      <c r="V3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15">
-      <c r="B4" s="79"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="59" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="74"/>
+      <c r="F4" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="59" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="59" t="s">
+      <c r="K4" s="74"/>
+      <c r="L4" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="59" t="s">
+      <c r="M4" s="74"/>
+      <c r="N4" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="59" t="s">
+      <c r="O4" s="74"/>
+      <c r="P4" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="59" t="s">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="S4" s="60"/>
-      <c r="T4" s="67"/>
-      <c r="V4" s="58"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="68"/>
+      <c r="V4" s="78"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="72" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="72" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="72" t="s">
+      <c r="G5" s="86"/>
+      <c r="H5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="72" t="s">
+      <c r="I5" s="86"/>
+      <c r="J5" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="73"/>
-      <c r="L5" s="72" t="s">
+      <c r="K5" s="86"/>
+      <c r="L5" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="72" t="s">
+      <c r="M5" s="86"/>
+      <c r="N5" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="O5" s="73"/>
-      <c r="P5" s="72" t="s">
+      <c r="O5" s="86"/>
+      <c r="P5" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="72" t="s">
+      <c r="Q5" s="86"/>
+      <c r="R5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="73"/>
-      <c r="T5" s="68"/>
-      <c r="V5" s="58"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="69"/>
+      <c r="V5" s="78"/>
     </row>
     <row r="6" spans="2:22">
       <c r="B6" s="14" t="s">
@@ -13022,20 +13024,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B2:T2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="T3:T5"/>
     <mergeCell ref="V3:V5"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="B3:B5"/>
@@ -13051,57 +13039,71 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="T3:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C196 T6:T196">
-    <cfRule type="expression" dxfId="24" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>$D$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576 Q1:Q1048576 S1:S1048576">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>$F$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>$H$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>$J$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>$R$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13143,121 +13145,121 @@
   <sheetData>
     <row r="1" spans="2:18" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="86"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:18" ht="15">
-      <c r="B3" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="45" t="s">
+      <c r="B3" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="59"/>
+      <c r="F3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="45" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="45" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="46"/>
-      <c r="N3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="82" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="57" t="s">
+      <c r="R3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15">
-      <c r="B4" s="79"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="59" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="74"/>
+      <c r="F4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="59" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="59" t="s">
+      <c r="K4" s="74"/>
+      <c r="L4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="59" t="s">
+      <c r="M4" s="74"/>
+      <c r="N4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="82"/>
-      <c r="R4" s="58"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="95"/>
+      <c r="R4" s="78"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="72" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="72" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="72" t="s">
+      <c r="G5" s="86"/>
+      <c r="H5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="72" t="s">
+      <c r="I5" s="86"/>
+      <c r="J5" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="73"/>
-      <c r="L5" s="72" t="s">
+      <c r="K5" s="86"/>
+      <c r="L5" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="72" t="s">
+      <c r="M5" s="86"/>
+      <c r="N5" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="73"/>
-      <c r="P5" s="83"/>
-      <c r="R5" s="58"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="96"/>
+      <c r="R5" s="78"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
@@ -16222,6 +16224,13 @@
     <sortCondition descending="1" ref="P6:P62"/>
   </sortState>
   <mergeCells count="23">
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="P3:P5"/>
@@ -16238,54 +16247,47 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C200 P6:P200">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>$D$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>$F$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>$H$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>$J$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>$L$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>$N$5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added mid-week results for week 4
</commit_message>
<xml_diff>
--- a/final/leaderboard.xlsx
+++ b/final/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meInspiron\Desktop\ipl_polls\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E961F7-6BA7-4B6E-9EBB-AF8EC978C3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146EA0DB-F1FB-496D-BF29-17A13E842FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{33315BC7-FE13-4B47-AD11-5FFBB64D564A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="247">
   <si>
     <t>Username</t>
   </si>
@@ -1515,6 +1515,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1542,24 +1569,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1567,15 +1576,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3629,43 +3629,43 @@
   <sheetData>
     <row r="1" spans="2:26" ht="5.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="66"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="75"/>
     </row>
     <row r="3" spans="2:26" ht="15" customHeight="1">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="79" t="s">
         <v>243</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="76" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="82" t="s">
+      <c r="D3" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="64" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="58" t="s">
@@ -3704,92 +3704,96 @@
         <v>231</v>
       </c>
       <c r="W3" s="59"/>
-      <c r="X3" s="67" t="s">
+      <c r="X3" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="77" t="s">
+      <c r="Z3" s="67" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26">
-      <c r="B4" s="71"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="73" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="73" t="s">
+      <c r="G4" s="70"/>
+      <c r="H4" s="69" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="73" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="69" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="73" t="s">
+      <c r="K4" s="70"/>
+      <c r="L4" s="69" t="s">
         <v>235</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="73" t="s">
+      <c r="M4" s="70"/>
+      <c r="N4" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="73" t="s">
+      <c r="O4" s="70"/>
+      <c r="P4" s="69" t="s">
         <v>237</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="73" t="s">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="69" t="s">
         <v>238</v>
       </c>
-      <c r="S4" s="74"/>
-      <c r="T4" s="73" t="s">
+      <c r="S4" s="70"/>
+      <c r="T4" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="U4" s="74"/>
-      <c r="V4" s="73" t="s">
+      <c r="U4" s="70"/>
+      <c r="V4" s="69" t="s">
         <v>240</v>
       </c>
-      <c r="W4" s="74"/>
-      <c r="X4" s="68"/>
-      <c r="Z4" s="78"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="77"/>
+      <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B5" s="72"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="75" t="s">
+      <c r="B5" s="81"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="75" t="s">
+      <c r="G5" s="72"/>
+      <c r="H5" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="76"/>
-      <c r="J5" s="75" t="s">
+      <c r="I5" s="72"/>
+      <c r="J5" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="75" t="s">
+      <c r="K5" s="72"/>
+      <c r="L5" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="75" t="s">
+      <c r="M5" s="72"/>
+      <c r="N5" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="76"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="76"/>
-      <c r="X5" s="69"/>
-      <c r="Z5" s="78"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="72"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="78"/>
+      <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="2:26">
       <c r="B6" s="42"/>
@@ -5272,6 +5276,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="X3:X5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="B2:X2"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
@@ -5288,24 +5310,6 @@
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="B2:X2"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:X5"/>
-    <mergeCell ref="D3:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:E100 X6:X100">
     <cfRule type="expression" dxfId="44" priority="14">
@@ -5441,7 +5445,7 @@
       <c r="B3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="64" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="58" t="s">
@@ -5487,55 +5491,55 @@
       <c r="X3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="77" t="s">
+      <c r="Z3" s="67" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="15">
       <c r="B4" s="92"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="69" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="73" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="73" t="s">
+      <c r="G4" s="70"/>
+      <c r="H4" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="73" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="73" t="s">
+      <c r="K4" s="70"/>
+      <c r="L4" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="73" t="s">
+      <c r="M4" s="70"/>
+      <c r="N4" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="73" t="s">
+      <c r="O4" s="70"/>
+      <c r="P4" s="69" t="s">
         <v>206</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="73" t="s">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="69" t="s">
         <v>207</v>
       </c>
-      <c r="S4" s="74"/>
-      <c r="T4" s="73" t="s">
+      <c r="S4" s="70"/>
+      <c r="T4" s="69" t="s">
         <v>208</v>
       </c>
-      <c r="U4" s="74"/>
-      <c r="V4" s="73" t="s">
+      <c r="U4" s="70"/>
+      <c r="V4" s="69" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="74"/>
-      <c r="X4" s="68"/>
-      <c r="Z4" s="78"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="77"/>
+      <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1">
       <c r="B5" s="93"/>
@@ -5580,8 +5584,8 @@
         <v>88</v>
       </c>
       <c r="W5" s="86"/>
-      <c r="X5" s="69"/>
-      <c r="Z5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="2:26">
       <c r="B6" s="14" t="s">
@@ -9402,28 +9406,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="Z3:Z5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="B2:X2"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
@@ -9437,6 +9419,28 @@
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="Z3:Z5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C194 X6:X194">
     <cfRule type="expression" dxfId="32" priority="46">
@@ -9569,7 +9573,7 @@
       <c r="B3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="64" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="58" t="s">
@@ -9607,47 +9611,47 @@
       <c r="T3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="77" t="s">
+      <c r="V3" s="67" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15">
       <c r="B4" s="92"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="69" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="73" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="73" t="s">
+      <c r="G4" s="70"/>
+      <c r="H4" s="69" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="73" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="73" t="s">
+      <c r="K4" s="70"/>
+      <c r="L4" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="73" t="s">
+      <c r="M4" s="70"/>
+      <c r="N4" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="O4" s="74"/>
-      <c r="P4" s="73" t="s">
+      <c r="O4" s="70"/>
+      <c r="P4" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="73" t="s">
+      <c r="Q4" s="70"/>
+      <c r="R4" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="S4" s="74"/>
-      <c r="T4" s="68"/>
-      <c r="V4" s="78"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="77"/>
+      <c r="V4" s="68"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1">
       <c r="B5" s="93"/>
@@ -9684,8 +9688,8 @@
         <v>17</v>
       </c>
       <c r="S5" s="86"/>
-      <c r="T5" s="69"/>
-      <c r="V5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="V5" s="68"/>
     </row>
     <row r="6" spans="2:22">
       <c r="B6" s="14" t="s">
@@ -13024,6 +13028,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="T3:T5"/>
     <mergeCell ref="V3:V5"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="B3:B5"/>
@@ -13039,20 +13057,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B2:T2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="T3:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C196 T6:T196">
     <cfRule type="expression" dxfId="19" priority="12">
@@ -13167,7 +13171,7 @@
       <c r="B3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="64" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="58" t="s">
@@ -13197,39 +13201,39 @@
       <c r="P3" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="77" t="s">
+      <c r="R3" s="67" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15">
       <c r="B4" s="92"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="73" t="s">
+      <c r="E4" s="70"/>
+      <c r="F4" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="73" t="s">
+      <c r="G4" s="70"/>
+      <c r="H4" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="73" t="s">
+      <c r="I4" s="70"/>
+      <c r="J4" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="73" t="s">
+      <c r="K4" s="70"/>
+      <c r="L4" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="73" t="s">
+      <c r="M4" s="70"/>
+      <c r="N4" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="74"/>
+      <c r="O4" s="70"/>
       <c r="P4" s="95"/>
-      <c r="R4" s="78"/>
+      <c r="R4" s="68"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1">
       <c r="B5" s="93"/>
@@ -13259,7 +13263,7 @@
       </c>
       <c r="O5" s="86"/>
       <c r="P5" s="96"/>
-      <c r="R5" s="78"/>
+      <c r="R5" s="68"/>
     </row>
     <row r="6" spans="2:18">
       <c r="B6" s="14" t="s">
@@ -16224,13 +16228,6 @@
     <sortCondition descending="1" ref="P6:P62"/>
   </sortState>
   <mergeCells count="23">
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="P3:P5"/>
@@ -16247,6 +16244,13 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C200 P6:P200">
     <cfRule type="expression" dxfId="8" priority="9">

</xml_diff>